<commit_message>
non-iid-U_SFL is not converge, the last accuracy is about 67.6.
</commit_message>
<xml_diff>
--- a/SFLV1 ResNet18 on HAM10000.xlsx
+++ b/SFLV1 ResNet18 on HAM10000.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="v1_test" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,10 +455,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>42.96604418073382</v>
+        <v>41.38967808314732</v>
       </c>
       <c r="C2" t="n">
-        <v>64.98263931274414</v>
+        <v>65.62500038146973</v>
       </c>
     </row>
     <row r="3">
@@ -466,10 +466,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>68.58935307094028</v>
+        <v>68.85213742937361</v>
       </c>
       <c r="C3" t="n">
-        <v>66.14583435058594</v>
+        <v>65.94618148803711</v>
       </c>
     </row>
     <row r="4">
@@ -477,10 +477,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>70.09807891845703</v>
+        <v>69.64556285313198</v>
       </c>
       <c r="C4" t="n">
-        <v>66.38454895019531</v>
+        <v>67.48263893127441</v>
       </c>
     </row>
     <row r="5">
@@ -488,10 +488,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>70.55262440272739</v>
+        <v>70.86816842215401</v>
       </c>
       <c r="C5" t="n">
-        <v>68.49392318725586</v>
+        <v>67.87326393127441</v>
       </c>
     </row>
     <row r="6">
@@ -499,13 +499,508 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>71.14245115007672</v>
+        <v>71.4820074898856</v>
       </c>
       <c r="C6" t="n">
-        <v>68.68055572509766</v>
+        <v>69.05382080078125</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>71.85403159005301</v>
+      </c>
+      <c r="C7" t="n">
+        <v>68.8975700378418</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>71.93080357142858</v>
+      </c>
+      <c r="C8" t="n">
+        <v>69.27517395019531</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>72.77800358363559</v>
+      </c>
+      <c r="C9" t="n">
+        <v>71.91406326293945</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>73.17809807913643</v>
+      </c>
+      <c r="C10" t="n">
+        <v>71.01996574401855</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>73.8051271711077</v>
+      </c>
+      <c r="C11" t="n">
+        <v>71.9053825378418</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>74.51670750209264</v>
+      </c>
+      <c r="C12" t="n">
+        <v>72.19183959960938</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>74.15347682407925</v>
+      </c>
+      <c r="C13" t="n">
+        <v>71.94010391235352</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>74.54579293387276</v>
+      </c>
+      <c r="C14" t="n">
+        <v>72.17447967529297</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>75.89251905168805</v>
+      </c>
+      <c r="C15" t="n">
+        <v>73.21614685058594</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>75.33380693708145</v>
+      </c>
+      <c r="C16" t="n">
+        <v>73.04253463745117</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>76.16680199759348</v>
+      </c>
+      <c r="C17" t="n">
+        <v>72.73871536254883</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>76.35010833740235</v>
+      </c>
+      <c r="C18" t="n">
+        <v>73.65451431274414</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>76.86925092424666</v>
+      </c>
+      <c r="C19" t="n">
+        <v>73.55902786254883</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>76.31595001220703</v>
+      </c>
+      <c r="C20" t="n">
+        <v>72.40017395019531</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>77.2747569492885</v>
+      </c>
+      <c r="C21" t="n">
+        <v>73.63715286254883</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>76.98356345040456</v>
+      </c>
+      <c r="C22" t="n">
+        <v>73.13368148803711</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>77.27205091203963</v>
+      </c>
+      <c r="C23" t="n">
+        <v>73.36805572509766</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>77.4381088256836</v>
+      </c>
+      <c r="C24" t="n">
+        <v>73.96701431274414</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>78.21158033098493</v>
+      </c>
+      <c r="C25" t="n">
+        <v>74.41840286254883</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>77.30113656180245</v>
+      </c>
+      <c r="C26" t="n">
+        <v>74.74826431274414</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>78.13852844238281</v>
+      </c>
+      <c r="C27" t="n">
+        <v>74.84375</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>78.93837956019811</v>
+      </c>
+      <c r="C28" t="n">
+        <v>74.24913177490234</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>78.17877458844866</v>
+      </c>
+      <c r="C29" t="n">
+        <v>74.17534790039062</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>79.44906681605748</v>
+      </c>
+      <c r="C30" t="n">
+        <v>74.26649322509766</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>79.40273284912109</v>
+      </c>
+      <c r="C31" t="n">
+        <v>73.26822967529297</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>79.0692642211914</v>
+      </c>
+      <c r="C32" t="n">
+        <v>75.09114608764648</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>79.41558467320033</v>
+      </c>
+      <c r="C33" t="n">
+        <v>74.80902786254883</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>79.36519230433873</v>
+      </c>
+      <c r="C34" t="n">
+        <v>74.70486221313476</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>79.4666532244001</v>
+      </c>
+      <c r="C35" t="n">
+        <v>74.55729217529297</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>79.30194832938056</v>
+      </c>
+      <c r="C36" t="n">
+        <v>73.7413200378418</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>79.61749223981585</v>
+      </c>
+      <c r="C37" t="n">
+        <v>73.9539924621582</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>79.71083613804409</v>
+      </c>
+      <c r="C38" t="n">
+        <v>74.70052185058594</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>80.48396933419365</v>
+      </c>
+      <c r="C39" t="n">
+        <v>74.59635467529297</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>81.26285204206195</v>
+      </c>
+      <c r="C40" t="n">
+        <v>74.88715362548828</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>80.20596596854072</v>
+      </c>
+      <c r="C41" t="n">
+        <v>74.24913177490234</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="n">
+        <v>80.27293025425503</v>
+      </c>
+      <c r="C42" t="n">
+        <v>73.3506950378418</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="n">
+        <v>81.55303061349051</v>
+      </c>
+      <c r="C43" t="n">
+        <v>74.07552185058594</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="n">
+        <v>81.56114741734098</v>
+      </c>
+      <c r="C44" t="n">
+        <v>74.75260391235352</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="n">
+        <v>81.1786392211914</v>
+      </c>
+      <c r="C45" t="n">
+        <v>74.93489608764648</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="n">
+        <v>81.1005142211914</v>
+      </c>
+      <c r="C46" t="n">
+        <v>75.35590286254883</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="n">
+        <v>81.28787907191685</v>
+      </c>
+      <c r="C47" t="n">
+        <v>74.05816040039062</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="n">
+        <v>81.72044132777623</v>
+      </c>
+      <c r="C48" t="n">
+        <v>74.4835075378418</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="n">
+        <v>82.33326612200055</v>
+      </c>
+      <c r="C49" t="n">
+        <v>74.52256927490234</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="n">
+        <v>82.19595533098493</v>
+      </c>
+      <c r="C50" t="n">
+        <v>74.9131950378418</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="n">
+        <v>82.68195386614119</v>
+      </c>
+      <c r="C51" t="n">
+        <v>75.3038200378418</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>